<commit_message>
update HTML, CSS, JS and images
</commit_message>
<xml_diff>
--- a/dataSets/MVPlayerOTY.xlsx
+++ b/dataSets/MVPlayerOTY.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kristopher Bognot\DSBootcamp\Project3Local\dataSets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Beau\Desktop\Bball\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865B4CF7-ACF2-4A98-8E14-3652CD1295A6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{46E1ECA7-DC63-4967-8780-B81038ABE7E5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10230" windowHeight="2860" xr2:uid="{D4D520BD-B48A-4D59-8725-76195FEB8AEA}"/>
   </bookViews>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="90">
+  <si>
+    <t>Season</t>
+  </si>
+  <si>
+    <t>Player</t>
+  </si>
   <si>
     <t>Age</t>
   </si>
@@ -68,251 +75,239 @@
     <t>FT%</t>
   </si>
   <si>
+    <t>2017-18</t>
+  </si>
+  <si>
+    <t>James Harden\hardeja01</t>
+  </si>
+  <si>
     <t>HOU</t>
   </si>
   <si>
+    <t>2016-17</t>
+  </si>
+  <si>
+    <t>Russell Westbrook\westbru01</t>
+  </si>
+  <si>
     <t>OKC</t>
   </si>
   <si>
+    <t>2015-16</t>
+  </si>
+  <si>
+    <t>Stephen Curry\curryst01</t>
+  </si>
+  <si>
     <t>GSW</t>
   </si>
   <si>
+    <t>2014-15</t>
+  </si>
+  <si>
+    <t>2013-14</t>
+  </si>
+  <si>
+    <t>Kevin Durant\duranke01</t>
+  </si>
+  <si>
+    <t>2012-13</t>
+  </si>
+  <si>
+    <t>LeBron James\jamesle01</t>
+  </si>
+  <si>
     <t>MIA</t>
   </si>
   <si>
+    <t>2011-12</t>
+  </si>
+  <si>
+    <t>2010-11</t>
+  </si>
+  <si>
+    <t>Derrick Rose\rosede01</t>
+  </si>
+  <si>
     <t>CHI</t>
   </si>
   <si>
+    <t>2009-10</t>
+  </si>
+  <si>
     <t>CLE</t>
   </si>
   <si>
+    <t>2008-09</t>
+  </si>
+  <si>
+    <t>2007-08</t>
+  </si>
+  <si>
+    <t>Kobe Bryant\bryanko01</t>
+  </si>
+  <si>
     <t>LAL</t>
   </si>
   <si>
+    <t>2006-07</t>
+  </si>
+  <si>
+    <t>Dirk Nowitzki\nowitdi01</t>
+  </si>
+  <si>
     <t>DAL</t>
   </si>
   <si>
+    <t>2005-06</t>
+  </si>
+  <si>
+    <t>Steve Nash\nashst01</t>
+  </si>
+  <si>
     <t>PHO</t>
   </si>
   <si>
+    <t>2004-05</t>
+  </si>
+  <si>
+    <t>2003-04</t>
+  </si>
+  <si>
+    <t>Kevin Garnett\garneke01</t>
+  </si>
+  <si>
     <t>MIN</t>
   </si>
   <si>
+    <t>2002-03</t>
+  </si>
+  <si>
+    <t>Tim Duncan\duncati01</t>
+  </si>
+  <si>
     <t>SAS</t>
   </si>
   <si>
+    <t>2001-02</t>
+  </si>
+  <si>
+    <t>2000-01</t>
+  </si>
+  <si>
+    <t>Allen Iverson\iversal01</t>
+  </si>
+  <si>
     <t>PHI</t>
   </si>
   <si>
+    <t>1999-00</t>
+  </si>
+  <si>
+    <t>Shaquille O'Neal\onealsh01</t>
+  </si>
+  <si>
+    <t>1998-99</t>
+  </si>
+  <si>
+    <t>Karl Malone\malonka01</t>
+  </si>
+  <si>
     <t>UTA</t>
   </si>
   <si>
+    <t>1997-98</t>
+  </si>
+  <si>
+    <t>Michael Jordan\jordami01</t>
+  </si>
+  <si>
+    <t>1996-97</t>
+  </si>
+  <si>
+    <t>1995-96</t>
+  </si>
+  <si>
+    <t>1994-95</t>
+  </si>
+  <si>
+    <t>David Robinson\robinda01</t>
+  </si>
+  <si>
+    <t>1993-94</t>
+  </si>
+  <si>
+    <t>Hakeem Olajuwon\olajuha01</t>
+  </si>
+  <si>
+    <t>1992-93</t>
+  </si>
+  <si>
+    <t>Charles Barkley\barklch01</t>
+  </si>
+  <si>
+    <t>1991-92</t>
+  </si>
+  <si>
+    <t>1990-91</t>
+  </si>
+  <si>
+    <t>1989-90</t>
+  </si>
+  <si>
+    <t>Magic Johnson\johnsma02</t>
+  </si>
+  <si>
+    <t>1988-89</t>
+  </si>
+  <si>
+    <t>1987-88</t>
+  </si>
+  <si>
+    <t>1986-87</t>
+  </si>
+  <si>
+    <t>1985-86</t>
+  </si>
+  <si>
+    <t>Larry Bird\birdla01</t>
+  </si>
+  <si>
     <t>BOS</t>
   </si>
   <si>
-    <t>2017</t>
-  </si>
-  <si>
-    <t>2016</t>
-  </si>
-  <si>
-    <t>2015</t>
-  </si>
-  <si>
-    <t>2014</t>
-  </si>
-  <si>
-    <t>2013</t>
-  </si>
-  <si>
-    <t>2012</t>
-  </si>
-  <si>
-    <t>2011</t>
-  </si>
-  <si>
-    <t>2010</t>
-  </si>
-  <si>
-    <t>2009</t>
-  </si>
-  <si>
-    <t>2008</t>
-  </si>
-  <si>
-    <t>2007</t>
-  </si>
-  <si>
-    <t>2006</t>
-  </si>
-  <si>
-    <t>2005</t>
-  </si>
-  <si>
-    <t>2004</t>
-  </si>
-  <si>
-    <t>2003</t>
-  </si>
-  <si>
-    <t>2002</t>
-  </si>
-  <si>
-    <t>2001</t>
-  </si>
-  <si>
-    <t>2000</t>
-  </si>
-  <si>
-    <t>1999</t>
-  </si>
-  <si>
-    <t>1998</t>
-  </si>
-  <si>
-    <t>1997</t>
-  </si>
-  <si>
-    <t>1996</t>
-  </si>
-  <si>
-    <t>1995</t>
-  </si>
-  <si>
-    <t>1994</t>
-  </si>
-  <si>
-    <t>1993</t>
-  </si>
-  <si>
-    <t>1992</t>
-  </si>
-  <si>
-    <t>1991</t>
-  </si>
-  <si>
-    <t>1990</t>
-  </si>
-  <si>
-    <t>1989</t>
-  </si>
-  <si>
-    <t>1988</t>
-  </si>
-  <si>
-    <t>1987</t>
-  </si>
-  <si>
-    <t>1986</t>
-  </si>
-  <si>
-    <t>1985</t>
-  </si>
-  <si>
-    <t>1984</t>
-  </si>
-  <si>
-    <t>1983</t>
-  </si>
-  <si>
-    <t>1982</t>
-  </si>
-  <si>
-    <t>1981</t>
-  </si>
-  <si>
-    <t>1980</t>
-  </si>
-  <si>
-    <t>1979</t>
-  </si>
-  <si>
-    <t>James Harden</t>
-  </si>
-  <si>
-    <t>Russell Westbrook</t>
-  </si>
-  <si>
-    <t>Stephen Curry</t>
-  </si>
-  <si>
-    <t>Kevin Durant</t>
-  </si>
-  <si>
-    <t>LeBron James</t>
-  </si>
-  <si>
-    <t>Derrick Rose</t>
-  </si>
-  <si>
-    <t>Kobe Bryant</t>
-  </si>
-  <si>
-    <t>Dirk Nowitzki</t>
-  </si>
-  <si>
-    <t>Steve Nash</t>
-  </si>
-  <si>
-    <t>Kevin Garnett</t>
-  </si>
-  <si>
-    <t>Tim Duncan</t>
-  </si>
-  <si>
-    <t>Allen Iverson</t>
-  </si>
-  <si>
-    <t>Shaquille O'Neal</t>
-  </si>
-  <si>
-    <t>Karl Malone</t>
-  </si>
-  <si>
-    <t>Michael Jordan</t>
-  </si>
-  <si>
-    <t>David Robinson</t>
-  </si>
-  <si>
-    <t>Hakeem Olajuwon</t>
-  </si>
-  <si>
-    <t>Charles Barkley</t>
-  </si>
-  <si>
-    <t>Magic Johnson</t>
-  </si>
-  <si>
-    <t>Larry Bird</t>
-  </si>
-  <si>
-    <t>Moses Malone</t>
-  </si>
-  <si>
-    <t>Julius Erving</t>
-  </si>
-  <si>
-    <t>Kareem Abdul-Jabbar</t>
-  </si>
-  <si>
-    <t>Award</t>
-  </si>
-  <si>
-    <t>MVP</t>
-  </si>
-  <si>
-    <t>Player</t>
-  </si>
-  <si>
-    <t>Year</t>
+    <t>1984-85</t>
+  </si>
+  <si>
+    <t>1983-84</t>
+  </si>
+  <si>
+    <t>1982-83</t>
+  </si>
+  <si>
+    <t>Moses Malone\malonmo01</t>
+  </si>
+  <si>
+    <t>1981-82</t>
+  </si>
+  <si>
+    <t>1980-81</t>
+  </si>
+  <si>
+    <t>Julius Erving\ervinju01</t>
+  </si>
+  <si>
+    <t>1979-80</t>
+  </si>
+  <si>
+    <t>Kareem Abdul-Jabbar\abdulka01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -665,76 +660,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{400D6491-EDB2-400C-BD1D-6CA895FA6929}">
-  <dimension ref="A1:O40"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="C2">
         <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E2">
         <v>72</v>
@@ -766,22 +755,19 @@
       <c r="N2">
         <v>0.85799999999999998</v>
       </c>
-      <c r="O2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E3">
         <v>81</v>
@@ -813,22 +799,19 @@
       <c r="N3">
         <v>0.84499999999999997</v>
       </c>
-      <c r="O3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="C4">
         <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E4">
         <v>79</v>
@@ -860,22 +843,19 @@
       <c r="N4">
         <v>0.90800000000000003</v>
       </c>
-      <c r="O4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="C5">
         <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E5">
         <v>80</v>
@@ -907,22 +887,19 @@
       <c r="N5">
         <v>0.91400000000000003</v>
       </c>
-      <c r="O5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="C6">
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E6">
         <v>81</v>
@@ -954,22 +931,19 @@
       <c r="N6">
         <v>0.873</v>
       </c>
-      <c r="O6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="C7">
         <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="E7">
         <v>76</v>
@@ -1001,22 +975,19 @@
       <c r="N7">
         <v>0.753</v>
       </c>
-      <c r="O7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="C8">
         <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="E8">
         <v>62</v>
@@ -1048,22 +1019,19 @@
       <c r="N8">
         <v>0.77100000000000002</v>
       </c>
-      <c r="O8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="C9">
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E9">
         <v>81</v>
@@ -1095,22 +1063,19 @@
       <c r="N9">
         <v>0.85799999999999998</v>
       </c>
-      <c r="O9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="C10">
         <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="E10">
         <v>76</v>
@@ -1142,22 +1107,19 @@
       <c r="N10">
         <v>0.76700000000000002</v>
       </c>
-      <c r="O10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="C11">
         <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="E11">
         <v>81</v>
@@ -1189,22 +1151,19 @@
       <c r="N11">
         <v>0.78</v>
       </c>
-      <c r="O11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="C12">
         <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="E12">
         <v>82</v>
@@ -1236,22 +1195,19 @@
       <c r="N12">
         <v>0.84</v>
       </c>
-      <c r="O12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="C13">
         <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="E13">
         <v>78</v>
@@ -1283,22 +1239,19 @@
       <c r="N13">
         <v>0.90400000000000003</v>
       </c>
-      <c r="O13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="C14">
         <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="E14">
         <v>79</v>
@@ -1330,22 +1283,19 @@
       <c r="N14">
         <v>0.92100000000000004</v>
       </c>
-      <c r="O14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="C15">
         <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="E15">
         <v>75</v>
@@ -1377,22 +1327,19 @@
       <c r="N15">
         <v>0.88700000000000001</v>
       </c>
-      <c r="O15" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="C16">
         <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="E16">
         <v>82</v>
@@ -1424,22 +1371,19 @@
       <c r="N16">
         <v>0.79100000000000004</v>
       </c>
-      <c r="O16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15">
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="C17">
         <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="E17">
         <v>81</v>
@@ -1471,22 +1415,19 @@
       <c r="N17">
         <v>0.71</v>
       </c>
-      <c r="O17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15">
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="C18">
         <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="E18">
         <v>82</v>
@@ -1518,22 +1459,19 @@
       <c r="N18">
         <v>0.79900000000000004</v>
       </c>
-      <c r="O18" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15">
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="C19">
         <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="E19">
         <v>71</v>
@@ -1565,22 +1503,19 @@
       <c r="N19">
         <v>0.81399999999999995</v>
       </c>
-      <c r="O19" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15">
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="C20">
         <v>27</v>
       </c>
       <c r="D20" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="E20">
         <v>79</v>
@@ -1612,22 +1547,19 @@
       <c r="N20">
         <v>0.52400000000000002</v>
       </c>
-      <c r="O20" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15">
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="C21">
         <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="E21">
         <v>49</v>
@@ -1659,22 +1591,19 @@
       <c r="N21">
         <v>0.78800000000000003</v>
       </c>
-      <c r="O21" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15">
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="C22">
         <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E22">
         <v>82</v>
@@ -1706,22 +1635,19 @@
       <c r="N22">
         <v>0.78400000000000003</v>
       </c>
-      <c r="O22" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15">
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="C23">
         <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="E23">
         <v>82</v>
@@ -1753,22 +1679,19 @@
       <c r="N23">
         <v>0.755</v>
       </c>
-      <c r="O23" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15">
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B24" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="C24">
         <v>32</v>
       </c>
       <c r="D24" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E24">
         <v>82</v>
@@ -1800,22 +1723,19 @@
       <c r="N24">
         <v>0.83399999999999996</v>
       </c>
-      <c r="O24" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15">
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="B25" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C25">
         <v>29</v>
       </c>
       <c r="D25" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="E25">
         <v>81</v>
@@ -1847,22 +1767,19 @@
       <c r="N25">
         <v>0.77400000000000002</v>
       </c>
-      <c r="O25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15">
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="C26">
         <v>31</v>
       </c>
       <c r="D26" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E26">
         <v>80</v>
@@ -1894,22 +1811,19 @@
       <c r="N26">
         <v>0.71599999999999997</v>
       </c>
-      <c r="O26" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15">
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="B27" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="C27">
         <v>29</v>
       </c>
       <c r="D27" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="E27">
         <v>76</v>
@@ -1941,22 +1855,19 @@
       <c r="N27">
         <v>0.76500000000000001</v>
       </c>
-      <c r="O27" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15">
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="B28" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="C28">
         <v>28</v>
       </c>
       <c r="D28" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E28">
         <v>80</v>
@@ -1988,22 +1899,19 @@
       <c r="N28">
         <v>0.83199999999999996</v>
       </c>
-      <c r="O28" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15">
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="B29" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="C29">
         <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E29">
         <v>82</v>
@@ -2035,22 +1943,19 @@
       <c r="N29">
         <v>0.85099999999999998</v>
       </c>
-      <c r="O29" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15">
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C30">
         <v>30</v>
       </c>
       <c r="D30" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="E30">
         <v>79</v>
@@ -2082,22 +1987,19 @@
       <c r="N30">
         <v>0.89</v>
       </c>
-      <c r="O30" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15">
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="B31" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C31">
         <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="E31">
         <v>77</v>
@@ -2129,22 +2031,19 @@
       <c r="N31">
         <v>0.91100000000000003</v>
       </c>
-      <c r="O31" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15">
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="B32" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="C32">
         <v>24</v>
       </c>
       <c r="D32" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E32">
         <v>82</v>
@@ -2176,22 +2075,19 @@
       <c r="N32">
         <v>0.84099999999999997</v>
       </c>
-      <c r="O32" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15">
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C33">
         <v>27</v>
       </c>
       <c r="D33" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="E33">
         <v>80</v>
@@ -2223,22 +2119,19 @@
       <c r="N33">
         <v>0.84799999999999998</v>
       </c>
-      <c r="O33" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15">
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="B34" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C34">
         <v>29</v>
       </c>
       <c r="D34" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="E34">
         <v>82</v>
@@ -2270,22 +2163,19 @@
       <c r="N34">
         <v>0.89600000000000002</v>
       </c>
-      <c r="O34" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15">
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="B35" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C35">
         <v>28</v>
       </c>
       <c r="D35" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="E35">
         <v>80</v>
@@ -2317,22 +2207,19 @@
       <c r="N35">
         <v>0.88200000000000001</v>
       </c>
-      <c r="O35" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15">
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="B36" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C36">
         <v>27</v>
       </c>
       <c r="D36" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="E36">
         <v>79</v>
@@ -2364,22 +2251,19 @@
       <c r="N36">
         <v>0.88800000000000001</v>
       </c>
-      <c r="O36" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15">
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="B37" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C37">
         <v>27</v>
       </c>
       <c r="D37" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="E37">
         <v>78</v>
@@ -2411,22 +2295,19 @@
       <c r="N37">
         <v>0.76100000000000001</v>
       </c>
-      <c r="O37" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15">
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="B38" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C38">
         <v>26</v>
       </c>
       <c r="D38" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E38">
         <v>81</v>
@@ -2458,22 +2339,19 @@
       <c r="N38">
         <v>0.76200000000000001</v>
       </c>
-      <c r="O38" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15">
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="B39" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C39">
         <v>30</v>
       </c>
       <c r="D39" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="E39">
         <v>82</v>
@@ -2505,22 +2383,19 @@
       <c r="N39">
         <v>0.78700000000000003</v>
       </c>
-      <c r="O39" t="s">
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B40" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15">
-      <c r="A40" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B40" t="s">
-        <v>87</v>
       </c>
       <c r="C40">
         <v>32</v>
       </c>
       <c r="D40" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="E40">
         <v>82</v>
@@ -2551,9 +2426,6 @@
       </c>
       <c r="N40">
         <v>0.76500000000000001</v>
-      </c>
-      <c r="O40" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>